<commit_message>
Label to excel + crop debugging
</commit_message>
<xml_diff>
--- a/Automation Data/Prototype_v2.5a.xlsx
+++ b/Automation Data/Prototype_v2.5a.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thak0\Documents\Year3_Intership_Application\Data Entry Automation\Repos\Data-Entry-Automation\Automation Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bottl\Desktop\Queuecut\GitHub\Data-Entry-Automation\Automation Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83C29B9-12C5-41CB-9364-F4BCE34AC2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D9CC9E-C50D-4E9B-B3F8-A0EDBBEA959F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="106">
   <si>
     <t>Category</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>Prawn</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
 </sst>
 </file>
@@ -888,10 +885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B18D7BF-B5FE-48F1-A6A6-774A6A382B57}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,11 +984,6 @@
       </c>
       <c r="C8" s="1" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Automationprocess and excel_generator for new excel format + debugging for img_preprocessing
</commit_message>
<xml_diff>
--- a/Automation Data/Prototype_v2.5a.xlsx
+++ b/Automation Data/Prototype_v2.5a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bottl\Desktop\Queuecut\GitHub\Data-Entry-Automation\Automation Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D9CC9E-C50D-4E9B-B3F8-A0EDBBEA959F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CE270E-7E57-4C27-B172-EE0AFD2EEE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,7 +739,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -888,7 +888,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,7 +996,7 @@
   <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>